<commit_message>
Change In Code Change-Id: I0000000000000000000000000000000000000003 Signed-off-by: Jaidip1994
</commit_message>
<xml_diff>
--- a/src/test/java/testData/DemoTestSuite.xlsx
+++ b/src/test/java/testData/DemoTestSuite.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I327559\git\DemoCode\src\test\java\testData\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="119">
   <si>
     <t>wait</t>
   </si>
@@ -80,24 +80,317 @@
     <t>Passed</t>
   </si>
   <si>
+    <t>toolsQAimg</t>
+  </si>
+  <si>
+    <t>xpath==.//img[contains(@src,'Tools-QA')]</t>
+  </si>
+  <si>
+    <t>exists</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>xpath==.//a[@title='Home']</t>
+  </si>
+  <si>
+    <t>xpath==.//a[@title='About us']</t>
+  </si>
+  <si>
+    <t>xpath==.//a[@title='Services']</t>
+  </si>
+  <si>
+    <t>xpath==.//a[@title='Demo']</t>
+  </si>
+  <si>
+    <t>xpath==.//a[@title='Blog']</t>
+  </si>
+  <si>
+    <t>xpath==.//a[@title='Contact']</t>
+  </si>
+  <si>
+    <t>homeTabMenu</t>
+  </si>
+  <si>
+    <t>servicesTabMenu</t>
+  </si>
+  <si>
+    <t>demoTabMenu</t>
+  </si>
+  <si>
+    <t>blogTabMenu</t>
+  </si>
+  <si>
+    <t>contactTabMenu</t>
+  </si>
+  <si>
     <t>aboutusTabMenu</t>
   </si>
   <si>
-    <t>xpath==.//a[@title='About us']</t>
-  </si>
-  <si>
-    <t>exists</t>
-  </si>
-  <si>
-    <t>tab</t>
+    <t>link</t>
+  </si>
+  <si>
+    <t>registrationNavMenu</t>
+  </si>
+  <si>
+    <t>xpath==.//h3[text()='Registration']/../..</t>
+  </si>
+  <si>
+    <t>interactionNavMenu</t>
+  </si>
+  <si>
+    <t>xpath==.//h3[text()='interaction']/../..</t>
+  </si>
+  <si>
+    <t>widgetNavMenu</t>
+  </si>
+  <si>
+    <t>xpath==.//h3[text()='Widget']/../..</t>
+  </si>
+  <si>
+    <t>framesandwinsNavMenu</t>
+  </si>
+  <si>
+    <t>xpath==.//h3[text()='Frames and Windows']/../..</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>scrollToBottom</t>
+  </si>
+  <si>
+    <t>scrollToTop</t>
+  </si>
+  <si>
+    <t>errorDivs</t>
+  </si>
+  <si>
+    <t>xpath==.//div[contains(@class,'error')]</t>
+  </si>
+  <si>
+    <t>verifyCountOfErrorDivs</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>divs</t>
+  </si>
+  <si>
+    <t>registrationLink</t>
+  </si>
+  <si>
+    <t>linkText==Registration</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>submitButton</t>
+  </si>
+  <si>
+    <t>xpath==.//input[@name='pie_submit']</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>takeScreenshot</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>countryDropdown</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Country']/../select</t>
+  </si>
+  <si>
+    <t>dobMonthDropdown</t>
+  </si>
+  <si>
+    <t>dobDayDropdown</t>
+  </si>
+  <si>
+    <t>dobYearDropdown</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Date of Birth']/..//select[contains(@id,'mm_date')]</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Date of Birth']/..//select[contains(@id,'dd_date')]</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Date of Birth']/..//select[contains(@id,'yy_date')]</t>
+  </si>
+  <si>
+    <t>firstnameInput</t>
+  </si>
+  <si>
+    <t>xpath==.//input[contains(@id,'firstname')]</t>
+  </si>
+  <si>
+    <t>lastnameInput</t>
+  </si>
+  <si>
+    <t>xpath==.//input[contains(@id,'lastname')]</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>textbox</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Hobby']/..//input</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Marital Status']/..//input</t>
+  </si>
+  <si>
+    <t>hobbyCheckboxList</t>
+  </si>
+  <si>
+    <t>maritalStatusRadioButtonList</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>radiobuttonlist</t>
+  </si>
+  <si>
+    <t>checkboxlist</t>
+  </si>
+  <si>
+    <t>cricket</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>clickRadioButtonWithGivenValue</t>
+  </si>
+  <si>
+    <t>clickCheckboxWithGivenValue</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>selectValue</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>phoneNumberInput</t>
+  </si>
+  <si>
+    <t>xpath==.//input[contains(@id,'phone')]</t>
+  </si>
+  <si>
+    <t>xpath==.//input[contains(@id,'username')]</t>
+  </si>
+  <si>
+    <t>userNameInput</t>
+  </si>
+  <si>
+    <t>FooAndBar</t>
+  </si>
+  <si>
+    <t>xpath==.//input[contains(@id,'email')]</t>
+  </si>
+  <si>
+    <t>emailInput</t>
+  </si>
+  <si>
+    <t>abc@xyz.to</t>
+  </si>
+  <si>
+    <t>aboutYourselfTextArea</t>
+  </si>
+  <si>
+    <t>xpath==.//textarea[contains(@id,'description')]</t>
+  </si>
+  <si>
+    <t>textarea</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Password']/..//input[contains(@id,'password')]</t>
+  </si>
+  <si>
+    <t>passwordInput</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>testautomation</t>
+  </si>
+  <si>
+    <t>xpath==.//label[text()='Confirm Password']/..//input[contains(@id,'password')]</t>
+  </si>
+  <si>
+    <t>confirmPasswordInput</t>
+  </si>
+  <si>
+    <t>automationTest</t>
+  </si>
+  <si>
+    <t>xpath==.//div[@id='password_meter']//div</t>
+  </si>
+  <si>
+    <t>passwordMatch</t>
+  </si>
+  <si>
+    <t>Mismatch</t>
+  </si>
+  <si>
+    <t>submitForm</t>
+  </si>
+  <si>
+    <t>xpath==.//input[@type='submit']</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>successMessageDialog</t>
+  </si>
+  <si>
+    <t>xpath==.//p[contains(text(),'Thank you')]</t>
+  </si>
+  <si>
+    <t>dialog</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>This is a test case for automation demo!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,12 +420,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -161,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -213,12 +500,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,20 +781,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H202"/>
+  <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="10" width="84.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="44.140625" collapsed="true"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="84.140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="44.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -558,15 +839,12 @@
       <c r="E2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A10" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -575,249 +853,715 @@
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
       <c r="E3" s="10">
-        <v>10000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+        <v>5000</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="2">
+        <f t="shared" ref="A11:A47" si="1">A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="E20" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="E24" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="C32" s="1"/>
+      <c r="H29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="10">
+        <v>2000</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1234567890</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="1"/>
+      <c r="A35" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="1"/>
+      <c r="A37" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="C40" s="1"/>
+      <c r="A40" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+      <c r="A41" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
+      <c r="A43" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>2000</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
       <c r="C46" s="1"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="C47" s="1"/>
+      <c r="A47" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
@@ -829,6 +1573,7 @@
       <c r="A52" s="2"/>
       <c r="C52" s="1"/>
       <c r="D52" s="3"/>
+      <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -840,19 +1585,23 @@
       <c r="A54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="20"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="C55" s="1"/>
       <c r="D55" s="3"/>
+      <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="C56" s="1"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="20"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -860,99 +1609,94 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="12"/>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="C61" s="1"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="C62" s="1"/>
       <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="12"/>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="C63" s="1"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="C64" s="1"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="C65" s="1"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="12"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="C66" s="1"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="14"/>
+      <c r="E66" s="12"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="C67" s="1"/>
       <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="C68" s="1"/>
       <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="14"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="C69" s="1"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="C71" s="1"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="9"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="C76" s="1"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="12"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="C77" s="1"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="13"/>
+      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
@@ -964,40 +1708,44 @@
       <c r="A79" s="2"/>
       <c r="C79" s="1"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="12"/>
+      <c r="E79" s="13"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="C80" s="1"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="11"/>
+      <c r="E80" s="12"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="C81" s="1"/>
       <c r="D81" s="3"/>
-      <c r="E81" s="11"/>
+      <c r="E81" s="12"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="C82" s="1"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="11"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="11"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="3"/>
-      <c r="E84"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
-      <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="C86" s="1"/>
+      <c r="D86" s="3"/>
+      <c r="E86"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
@@ -1006,12 +1754,10 @@
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="C88" s="1"/>
-      <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="C89" s="1"/>
-      <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
@@ -1021,20 +1767,22 @@
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="C91" s="1"/>
+      <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
+      <c r="C92" s="1"/>
+      <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
-      <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
-      <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
@@ -1042,6 +1790,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
+      <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
@@ -1049,22 +1798,21 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
-      <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
+      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
-      <c r="E101"/>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
-      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
-      <c r="C103" s="1"/>
+      <c r="E103"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
@@ -1076,18 +1824,18 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
-      <c r="E107"/>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
-      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
-      <c r="C109" s="1"/>
+      <c r="E109"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
@@ -1099,18 +1847,18 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
+      <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
-      <c r="E113"/>
+      <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
-      <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
-      <c r="C115" s="1"/>
+      <c r="E115"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
@@ -1122,35 +1870,37 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
+      <c r="C118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
+      <c r="C119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
-      <c r="C120" s="1"/>
-    </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
     </row>
-    <row r="122" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
-    </row>
-    <row r="123" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
-      <c r="C125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
+      <c r="C127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
@@ -1160,20 +1910,20 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
-      <c r="E130"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
-      <c r="D132" s="3"/>
+      <c r="E132"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
+      <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
@@ -1379,9 +2129,18 @@
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
     </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E36" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1391,17 +2150,17 @@
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="10" width="84.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="44.140625" collapsed="true"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="84.140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="44.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1463,7 +2222,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
       <c r="E3" s="10">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -2254,11 +3013,8 @@
       <c r="A201" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" location="Shell-home" display="https://fbt.wdf.sap.corp:44390/sap/bc/ui5_ui5/ui2/ushell/shells/abap/FioriLaunchpad.html - Shell-home"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2267,17 +3023,17 @@
   <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="10" width="96.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="67.0" collapsed="true"/>
+    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="96.140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="67" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2339,7 +3095,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
       <c r="E3" s="10">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -2453,14 +3209,14 @@
   <dimension ref="A1:C133"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="208.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="208" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2475,109 +3231,252 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>

</xml_diff>

<commit_message>
Change in the code
Change-Id: I0000000000000000000000000000000000000006
Signed-off-by: Jaidip1994
</commit_message>
<xml_diff>
--- a/src/test/java/testData/DemoTestSuite.xlsx
+++ b/src/test/java/testData/DemoTestSuite.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I327559\git\DemoCode\src\test\java\testData\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="150">
   <si>
     <t>wait</t>
   </si>
@@ -362,18 +362,12 @@
     <t>xpath==.//input[@type='submit']</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
     <t>successMessageDialog</t>
   </si>
   <si>
     <t>xpath==.//p[contains(text(),'Thank you')]</t>
   </si>
   <si>
-    <t>dialog</t>
-  </si>
-  <si>
     <t>clear</t>
   </si>
   <si>
@@ -384,12 +378,112 @@
   </si>
   <si>
     <t>This is a test case for automation demo!</t>
+  </si>
+  <si>
+    <t>linkText==Draggable</t>
+  </si>
+  <si>
+    <t>draggableLink</t>
+  </si>
+  <si>
+    <t>dragElement</t>
+  </si>
+  <si>
+    <t>xpath==.//div[@id='draggable']/p</t>
+  </si>
+  <si>
+    <t>dragNDrop</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>dragTo</t>
+  </si>
+  <si>
+    <t>xpath==.//div[@class='inside_contain']</t>
+  </si>
+  <si>
+    <t>linkText==Constrain movement</t>
+  </si>
+  <si>
+    <t>constrainMovLink</t>
+  </si>
+  <si>
+    <t>xpath==.//p[contains(text(),'vertically')]</t>
+  </si>
+  <si>
+    <t>verticallyDragTile</t>
+  </si>
+  <si>
+    <t>dragNDropByOffset</t>
+  </si>
+  <si>
+    <t>tile</t>
+  </si>
+  <si>
+    <t>horizontallyDragTile</t>
+  </si>
+  <si>
+    <t>xpath==.//p[contains(text(),'horizontally')]</t>
+  </si>
+  <si>
+    <t>0,-100</t>
+  </si>
+  <si>
+    <t>0,+200</t>
+  </si>
+  <si>
+    <t>-200,0</t>
+  </si>
+  <si>
+    <t>300,0</t>
+  </si>
+  <si>
+    <t>linkText==Autocomplete</t>
+  </si>
+  <si>
+    <t>autoCompleteLink</t>
+  </si>
+  <si>
+    <t>scrollForEle</t>
+  </si>
+  <si>
+    <t>xpath==.//input[@id='tagss']</t>
+  </si>
+  <si>
+    <t>tagsInput</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>selectFromDropDwnClick</t>
+  </si>
+  <si>
+    <t>xpath==.//ul[contains(@class,'ui-autocomplete')]</t>
+  </si>
+  <si>
+    <t>tagsDropDown</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>No Action to be processed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -781,20 +875,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H204"/>
+  <dimension ref="A1:H207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G47"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="84.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="44.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="10" width="84.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="44.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -839,6 +933,9 @@
       <c r="E2" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
@@ -855,6 +952,9 @@
       <c r="E3" s="10">
         <v>5000</v>
       </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
@@ -872,6 +972,9 @@
       <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -888,6 +991,9 @@
       <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -904,6 +1010,9 @@
       <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -920,6 +1029,9 @@
       <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -936,6 +1048,9 @@
       <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,6 +1067,9 @@
       <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,10 +1086,13 @@
       <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" ref="A11:A47" si="1">A10+1</f>
+        <f t="shared" ref="A11:A63" si="1">A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -983,6 +1104,9 @@
       <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -998,6 +1122,9 @@
       <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1007,6 +1134,9 @@
       <c r="B13" t="s">
         <v>43</v>
       </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1022,6 +1152,9 @@
       <c r="D14" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1037,6 +1170,9 @@
       <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1048,6 +1184,9 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1063,6 +1202,9 @@
       <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -1070,13 +1212,15 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1085,7 +1229,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1094,12 +1247,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="10">
-        <v>7</v>
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1108,16 +1259,15 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="10">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1126,16 +1276,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>72</v>
+        <v>49</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1147,13 +1300,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1162,12 +1318,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E24" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1176,16 +1339,15 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H25" t="s">
-        <v>57</v>
+        <v>83</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1194,10 +1356,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1206,12 +1377,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="10" t="s">
-        <v>81</v>
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1220,16 +1392,15 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" t="s">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1238,12 +1409,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
       <c r="H29" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1252,16 +1430,15 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="1"/>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1273,13 +1450,16 @@
         <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="10">
-        <v>1</v>
+      <c r="E31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1291,7 +1471,7 @@
         <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>85</v>
@@ -1299,8 +1479,11 @@
       <c r="E32" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -1309,34 +1492,40 @@
         <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="10">
         <v>2000</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="10">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -1345,16 +1534,19 @@
         <v>70</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="10">
+        <v>1234567890</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1363,16 +1555,19 @@
         <v>70</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1381,16 +1576,19 @@
         <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -1399,16 +1597,19 @@
         <v>70</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -1417,55 +1618,67 @@
         <v>70</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E41" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>104</v>
@@ -1473,164 +1686,405 @@
       <c r="D42" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E43" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="E44" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="3"/>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>0</v>
       </c>
-      <c r="E44" s="10">
+      <c r="C47" s="1"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="10">
         <v>2000</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>0</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+      <c r="E51" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
       <c r="C53" s="1"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+      <c r="E53" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="20"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
+      <c r="E56" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="20"/>
+      <c r="F59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>0</v>
+      </c>
       <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="12"/>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="3"/>
+      <c r="E60" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F61" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="C64" s="1"/>
       <c r="D64" s="3"/>
@@ -1639,82 +2093,80 @@
       <c r="A65" s="2"/>
       <c r="C65" s="1"/>
       <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="C66" s="1"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="C67" s="1"/>
       <c r="D67" s="3"/>
-      <c r="E67" s="12"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="C68" s="1"/>
       <c r="D68" s="3"/>
-      <c r="E68" s="14"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="C69" s="1"/>
       <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="12"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="C70" s="1"/>
       <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="C71" s="1"/>
       <c r="D71" s="3"/>
+      <c r="E71" s="14"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="1"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="12"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="C79" s="1"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="13"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="C80" s="1"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="12"/>
+      <c r="E80" s="9"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
@@ -1726,26 +2178,31 @@
       <c r="A82" s="2"/>
       <c r="C82" s="1"/>
       <c r="D82" s="3"/>
-      <c r="E82" s="11"/>
+      <c r="E82" s="13"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="C83" s="1"/>
       <c r="D83" s="3"/>
-      <c r="E83" s="11"/>
+      <c r="E83" s="12"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="C84" s="1"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="12"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="11"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="C86" s="1"/>
       <c r="D86" s="3"/>
-      <c r="E86"/>
+      <c r="E86" s="11"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
@@ -1753,36 +2210,39 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
-      <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="C89" s="1"/>
+      <c r="D89" s="3"/>
+      <c r="E89"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="C90" s="1"/>
-      <c r="E90" s="11"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="C91" s="1"/>
-      <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="C92" s="1"/>
-      <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="C93" s="1"/>
+      <c r="E93" s="11"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
+      <c r="C94" s="1"/>
+      <c r="E94" s="11"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
+      <c r="C95" s="1"/>
+      <c r="E95" s="11"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
@@ -1790,14 +2250,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
-      <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
-      <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
+      <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
@@ -1812,7 +2271,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
-      <c r="E103"/>
+      <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
@@ -1820,11 +2279,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
-      <c r="C105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
-      <c r="C106" s="1"/>
+      <c r="E106"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
@@ -1832,10 +2290,11 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
+      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
-      <c r="E109"/>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
@@ -1843,11 +2302,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
-      <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
-      <c r="C112" s="1"/>
+      <c r="E112"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
@@ -1855,10 +2313,11 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
+      <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
-      <c r="E115"/>
+      <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
@@ -1866,11 +2325,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
-      <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
-      <c r="C118" s="1"/>
+      <c r="E118"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
@@ -1878,31 +2336,33 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
+      <c r="C120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
+      <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
     </row>
-    <row r="124" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
-      <c r="C127" s="1"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,29 +2370,30 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
+      <c r="C130" s="1"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
-      <c r="E132"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
-      <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
+      <c r="E135"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
+      <c r="D137" s="3"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
@@ -2135,9 +2596,18 @@
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
     </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E36" r:id="rId1"/>
+    <hyperlink ref="E37" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId2"/>
@@ -2155,12 +2625,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="84.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="44.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="10" width="84.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="44.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3028,12 +3498,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="96.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="67" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="10" width="96.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="67.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3208,15 +3678,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A16" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="208" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="208.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3472,41 +3942,83 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>

</xml_diff>